<commit_message>
checks of dynalene data in dec/IncompressibleLiquids/Dynalene_manufacturer_data.xlsx
Signed-off-by: Ian Bell <ian.h.bell@gmail.com>
</commit_message>
<xml_diff>
--- a/dev/IncompressibleLiquids/Dynalene_manufacturer_data.xlsx
+++ b/dev/IncompressibleLiquids/Dynalene_manufacturer_data.xlsx
@@ -83,6 +83,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5457,15 +5462,15 @@
   <dimension ref="A2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -5540,15 +5545,15 @@
         <f>[1]!Props("V","T",G3+0.01,"P",101,"DynaleneHC-50")</f>
         <v>34730.138835519167</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <f>[1]!Props("L","T",G3+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.3496897303748302E-7</v>
-      </c>
-      <c r="O3">
+        <v>0.434968973037483</v>
+      </c>
+      <c r="O3" s="1">
         <f>[1]!Props("C","T",G3+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.5625137584888784</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <f>[1]!Props("D","T",G3+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1378.2459075109136</v>
       </c>
@@ -5593,15 +5598,15 @@
         <f>[1]!Props("V","T",G4+0.01,"P",101,"DynaleneHC-50")</f>
         <v>20346.909069221703</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <f>[1]!Props("L","T",G4+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.449821095025505E-7</v>
-      </c>
-      <c r="O4">
+        <v>0.4449821095025504</v>
+      </c>
+      <c r="O4" s="1">
         <f>[1]!Props("C","T",G4+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.5824058110945765</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <f>[1]!Props("D","T",G4+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1372.7363231624058</v>
       </c>
@@ -5646,15 +5651,15 @@
         <f>[1]!Props("V","T",G5+0.01,"P",101,"DynaleneHC-50")</f>
         <v>13100.862472709419</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <f>[1]!Props("L","T",G5+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.5499387761817312E-7</v>
-      </c>
-      <c r="O5">
+        <v>0.45499387761817311</v>
+      </c>
+      <c r="O5" s="1">
         <f>[1]!Props("C","T",G5+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.6022582072271114</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="2">
         <f>[1]!Props("D","T",G5+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1367.2211057400382</v>
       </c>
@@ -5699,15 +5704,15 @@
         <f>[1]!Props("V","T",G6+0.01,"P",101,"DynaleneHC-50")</f>
         <v>9060.0060551075912</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <f>[1]!Props("L","T",G6+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.6500427738435094E-7</v>
-      </c>
-      <c r="O6">
+        <v>0.46500427738435091</v>
+      </c>
+      <c r="O6" s="1">
         <f>[1]!Props("C","T",G6+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.6220742828021946</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="2">
         <f>[1]!Props("D","T",G6+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1361.7006285615003</v>
       </c>
@@ -5752,15 +5757,15 @@
         <f>[1]!Props("V","T",G7+0.01,"P",101,"DynaleneHC-50")</f>
         <v>6622.1430200941968</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <f>[1]!Props("L","T",G7+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.75013308801084E-7</v>
-      </c>
-      <c r="O7">
+        <v>0.47501330880108394</v>
+      </c>
+      <c r="O7" s="1">
         <f>[1]!Props("C","T",G7+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.6418573737355353</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="2">
         <f>[1]!Props("D","T",G7+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1356.1752649444823</v>
       </c>
@@ -5805,15 +5810,15 @@
         <f>[1]!Props("V","T",G8+0.01,"P",101,"DynaleneHC-50")</f>
         <v>5056.7919624258593</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <f>[1]!Props("L","T",G8+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.8502097186837221E-7</v>
-      </c>
-      <c r="O8">
+        <v>0.48502097186837223</v>
+      </c>
+      <c r="O8" s="1">
         <f>[1]!Props("C","T",G8+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.6616108159428467</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="2">
         <f>[1]!Props("D","T",G8+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1350.6453882066739</v>
       </c>
@@ -5858,15 +5863,15 @@
         <f>[1]!Props("V","T",G9+0.01,"P",101,"DynaleneHC-50")</f>
         <v>3999.7910504116116</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <f>[1]!Props("L","T",G9+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>4.9502726658621566E-7</v>
-      </c>
-      <c r="O9">
+        <v>0.49502726658621565</v>
+      </c>
+      <c r="O9" s="1">
         <f>[1]!Props("C","T",G9+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.6813379453398385</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="2">
         <f>[1]!Props("D","T",G9+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1345.1113716657651</v>
       </c>
@@ -5911,15 +5916,15 @@
         <f>[1]!Props("V","T",G10+0.01,"P",101,"DynaleneHC-50")</f>
         <v>3255.9380262721224</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <f>[1]!Props("L","T",G10+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.0503219295461431E-7</v>
-      </c>
-      <c r="O10">
+        <v>0.50503219295461432</v>
+      </c>
+      <c r="O10" s="1">
         <f>[1]!Props("C","T",G10+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.701042097842222</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="2">
         <f>[1]!Props("D","T",G10+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1339.5735886394455</v>
       </c>
@@ -5964,15 +5969,15 @@
         <f>[1]!Props("V","T",G11+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2714.1326002447913</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <f>[1]!Props("L","T",G11+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.1503575097356816E-7</v>
-      </c>
-      <c r="O11">
+        <v>0.51503575097356813</v>
+      </c>
+      <c r="O11" s="1">
         <f>[1]!Props("C","T",G11+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.7207266093657085</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="2">
         <f>[1]!Props("D","T",G11+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1334.0324124454048</v>
       </c>
@@ -6017,15 +6022,15 @@
         <f>[1]!Props("V","T",G12+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2307.8798956998639</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <f>[1]!Props("L","T",G12+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.2503794064307719E-7</v>
-      </c>
-      <c r="O12">
+        <v>0.52503794064307729</v>
+      </c>
+      <c r="O12" s="1">
         <f>[1]!Props("C","T",G12+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.7403948158260092</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="2">
         <f>[1]!Props("D","T",G12+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1328.4882164013331</v>
       </c>
@@ -6070,15 +6075,15 @@
         <f>[1]!Props("V","T",G13+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1995.6448089217342</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <f>[1]!Props("L","T",G13+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.3503876196314143E-7</v>
-      </c>
-      <c r="O13">
+        <v>0.53503876196314137</v>
+      </c>
+      <c r="O13" s="1">
         <f>[1]!Props("C","T",G13+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.7600500531388343</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="2">
         <f>[1]!Props("D","T",G13+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1322.9413738249204</v>
       </c>
@@ -6123,15 +6128,15 @@
         <f>[1]!Props("V","T",G14+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1750.5134964010153</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <f>[1]!Props("L","T",G14+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.4503821493376096E-7</v>
-      </c>
-      <c r="O14">
+        <v>0.54503821493376081</v>
+      </c>
+      <c r="O14" s="1">
         <f>[1]!Props("C","T",G14+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.7796956572198956</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="2">
         <f>[1]!Props("D","T",G14+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1317.3922580338563</v>
       </c>
@@ -6176,15 +6181,15 @@
         <f>[1]!Props("V","T",G15+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1554.482757924221</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <f>[1]!Props("L","T",G15+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.5503629955493559E-7</v>
-      </c>
-      <c r="O15">
+        <v>0.55503629955493561</v>
+      </c>
+      <c r="O15" s="1">
         <f>[1]!Props("C","T",G15+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.7993349639849039</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="2">
         <f>[1]!Props("D","T",G15+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1311.8412423458306</v>
       </c>
@@ -6229,15 +6234,15 @@
         <f>[1]!Props("V","T",G16+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1395.1703169069121</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="1">
         <f>[1]!Props("L","T",G16+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.6503301582666541E-7</v>
-      </c>
-      <c r="O16">
+        <v>0.56503301582666543</v>
+      </c>
+      <c r="O16" s="1">
         <f>[1]!Props("C","T",G16+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.8189713093495703</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="2">
         <f>[1]!Props("D","T",G16+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1306.2887000785331</v>
       </c>
@@ -6282,15 +6287,15 @@
         <f>[1]!Props("V","T",G17+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1263.8486948203636</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="1">
         <f>[1]!Props("L","T",G17+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.7502836374895042E-7</v>
-      </c>
-      <c r="O17">
+        <v>0.57502836374895039</v>
+      </c>
+      <c r="O17" s="1">
         <f>[1]!Props("C","T",G17+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.8386080292296056</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="2">
         <f>[1]!Props("D","T",G17+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1300.7350045496537</v>
       </c>
@@ -6335,15 +6340,15 @@
         <f>[1]!Props("V","T",G18+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1154.2313815724306</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="1">
         <f>[1]!Props("L","T",G18+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.8502234332179063E-7</v>
-      </c>
-      <c r="O18">
+        <v>0.58502234332179071</v>
+      </c>
+      <c r="O18" s="1">
         <f>[1]!Props("C","T",G18+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.8582484595407207</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="2">
         <f>[1]!Props("D","T",G18+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1295.1805290768823</v>
       </c>
@@ -6388,15 +6393,15 @@
         <f>[1]!Props("V","T",G19+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1061.7015353790705</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="1">
         <f>[1]!Props("L","T",G19+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>5.9501495454518604E-7</v>
-      </c>
-      <c r="O19">
+        <v>0.59501495454518616</v>
+      </c>
+      <c r="O19" s="1">
         <f>[1]!Props("C","T",G19+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.8778959361986276</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="2">
         <f>[1]!Props("D","T",G19+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1289.6256469779084</v>
       </c>
@@ -6441,15 +6446,15 @@
         <f>[1]!Props("V","T",G20+0.01,"P",101,"DynaleneHC-50")</f>
         <v>982.80908716865133</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <f>[1]!Props("L","T",G20+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.0500619741913674E-7</v>
-      </c>
-      <c r="O20">
+        <v>0.60500619741913675</v>
+      </c>
+      <c r="O20" s="1">
         <f>[1]!Props("C","T",G20+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.8975537951190362</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="2">
         <f>[1]!Props("D","T",G20+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1284.0707315704226</v>
       </c>
@@ -6494,15 +6499,15 @@
         <f>[1]!Props("V","T",G21+0.01,"P",101,"DynaleneHC-50")</f>
         <v>914.93516729156738</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="1">
         <f>[1]!Props("L","T",G21+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.1499607194364264E-7</v>
-      </c>
-      <c r="O21">
+        <v>0.61499607194364259</v>
+      </c>
+      <c r="O21" s="1">
         <f>[1]!Props("C","T",G21+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.9172253722176587</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="2">
         <f>[1]!Props("D","T",G21+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1278.5161561721138</v>
       </c>
@@ -6547,15 +6552,15 @@
         <f>[1]!Props("V","T",G22+0.01,"P",101,"DynaleneHC-50")</f>
         <v>856.06345161942045</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <f>[1]!Props("L","T",G22+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.2498457811870363E-7</v>
-      </c>
-      <c r="O22">
+        <v>0.62498457811870367</v>
+      </c>
+      <c r="O22" s="1">
         <f>[1]!Props("C","T",G22+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.9369140034102053</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="2">
         <f>[1]!Props("D","T",G22+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1272.9622941006726</v>
       </c>
@@ -6600,15 +6605,15 @@
         <f>[1]!Props("V","T",G23+0.01,"P",101,"DynaleneHC-50")</f>
         <v>804.62137645317705</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="1">
         <f>[1]!Props("L","T",G23+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.3497171594431992E-7</v>
-      </c>
-      <c r="O23">
+        <v>0.63497171594431989</v>
+      </c>
+      <c r="O23" s="1">
         <f>[1]!Props("C","T",G23+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.9566230246123868</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="2">
         <f>[1]!Props("D","T",G23+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1267.4095186737882</v>
       </c>
@@ -6653,15 +6658,15 @@
         <f>[1]!Props("V","T",G24+0.01,"P",101,"DynaleneHC-50")</f>
         <v>759.36795008276488</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="1">
         <f>[1]!Props("L","T",G24+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.449574854204913E-7</v>
-      </c>
-      <c r="O24">
+        <v>0.64495748542049136</v>
+      </c>
+      <c r="O24" s="1">
         <f>[1]!Props("C","T",G24+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.9763557717399149</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="2">
         <f>[1]!Props("D","T",G24+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1261.858203209151</v>
       </c>
@@ -6706,15 +6711,15 @@
         <f>[1]!Props("V","T",G25+0.01,"P",101,"DynaleneHC-50")</f>
         <v>719.31322375850766</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="1">
         <f>[1]!Props("L","T",G25+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.5494188654721799E-7</v>
-      </c>
-      <c r="O25">
+        <v>0.65494188654721797</v>
+      </c>
+      <c r="O25" s="1">
         <f>[1]!Props("C","T",G25+0.01,"P",101,"DynaleneHC-50")</f>
         <v>2.9961155807085005</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="2">
         <f>[1]!Props("D","T",G25+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1256.3087210244503</v>
       </c>
@@ -6759,15 +6764,15 @@
         <f>[1]!Props("V","T",G26+0.01,"P",101,"DynaleneHC-50")</f>
         <v>683.65964299528639</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <f>[1]!Props("L","T",G26+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.6492491932449986E-7</v>
-      </c>
-      <c r="O26">
+        <v>0.66492491932449982</v>
+      </c>
+      <c r="O26" s="1">
         <f>[1]!Props("C","T",G26+0.01,"P",101,"DynaleneHC-50")</f>
         <v>3.0159057874338546</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="2">
         <f>[1]!Props("D","T",G26+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1250.7614454373763</v>
       </c>
@@ -6812,15 +6817,15 @@
         <f>[1]!Props("V","T",G27+0.01,"P",101,"DynaleneHC-50")</f>
         <v>651.75875966300316</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="1">
         <f>[1]!Props("L","T",G27+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.7490658375233693E-7</v>
-      </c>
-      <c r="O27">
+        <v>0.67490658375233692</v>
+      </c>
+      <c r="O27" s="1">
         <f>[1]!Props("C","T",G27+0.01,"P",101,"DynaleneHC-50")</f>
         <v>3.0357297278316882</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="2">
         <f>[1]!Props("D","T",G27+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1245.2167497656189</v>
       </c>
@@ -6865,15 +6870,15 @@
         <f>[1]!Props("V","T",G28+0.01,"P",101,"DynaleneHC-50")</f>
         <v>623.07888501033665</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="1">
         <f>[1]!Props("L","T",G28+0.01,"P",101,"DynaleneHC-50")</f>
-        <v>6.8488687983072909E-7</v>
-      </c>
-      <c r="O28">
+        <v>0.68488687983072905</v>
+      </c>
+      <c r="O28" s="1">
         <f>[1]!Props("C","T",G28+0.01,"P",101,"DynaleneHC-50")</f>
         <v>3.0555907378177123</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="2">
         <f>[1]!Props("D","T",G28+0.01,"P",101,"DynaleneHC-50")</f>
         <v>1239.6750073268677</v>
       </c>

</xml_diff>